<commit_message>
new edits to spreadsheet
</commit_message>
<xml_diff>
--- a/BarGraphsofData.xlsx
+++ b/BarGraphsofData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramyanataraj/Documents/Spring 2025/IC25/DC-WMATA-Metro-Ridership/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECF2821B-8DD3-3745-8F59-402170AFE412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4538112E-8D59-C143-B6DB-00FD8B69770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="800" windowWidth="28040" windowHeight="17440" xr2:uid="{7288D198-DE04-1C48-9B79-CFC36871A335}"/>
+    <workbookView xWindow="11760" yWindow="780" windowWidth="19060" windowHeight="17440" xr2:uid="{7288D198-DE04-1C48-9B79-CFC36871A335}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Indexes</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>June</t>
+  </si>
+  <si>
+    <t>De cember</t>
   </si>
 </sst>
 </file>
@@ -276,7 +279,15 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Weekend</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Weekend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -294,16 +305,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>September</c:v>
+                  <c:v>March</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>March</c:v>
+                  <c:v>June</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>September</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>June</c:v>
+                  <c:v>De cember</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -315,16 +326,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>202700</c:v>
+                  <c:v>242500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>261700</c:v>
+                  <c:v>282200</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>289600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>282200</c:v>
+                  <c:v>202700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -365,16 +376,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>September</c:v>
+                  <c:v>March</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>March</c:v>
+                  <c:v>June</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>September</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>June</c:v>
+                  <c:v>De cember</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -386,16 +397,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>432100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>452600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>427700</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>454700</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>432100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>381000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>452600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,10 +754,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>259050</c:v>
+                  <c:v>271433.33333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>430100</c:v>
+                  <c:v>437466.66666666669</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1015,7 +1026,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$2</c:f>
+              <c:f>Sheet1!$W$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -1033,30 +1044,30 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$3:$R$7</c:f>
+              <c:f>Sheet1!$V$3:$V$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Evening (7pm-12am)</c:v>
+                  <c:v>AM Peak (Open-9:30am)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Late Night (12am-Close)</c:v>
+                  <c:v>Midday (9:30am-3pm)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>PM Peak (3pm-7pm)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Midday (9:30am-3pm)</c:v>
+                  <c:v>Evening (7pm-12am)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>AM Peak (Open-9:30am)</c:v>
+                  <c:v>Late Night (12am-Close)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$3:$S$7</c:f>
+              <c:f>Sheet1!$W$3:$W$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1074,7 +1085,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$2</c:f>
+              <c:f>Sheet1!$X$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1095,47 +1106,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$3:$R$7</c:f>
+              <c:f>Sheet1!$V$3:$V$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Evening (7pm-12am)</c:v>
+                  <c:v>AM Peak (Open-9:30am)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Late Night (12am-Close)</c:v>
+                  <c:v>Midday (9:30am-3pm)</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>PM Peak (3pm-7pm)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Midday (9:30am-3pm)</c:v>
+                  <c:v>Evening (7pm-12am)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>AM Peak (Open-9:30am)</c:v>
+                  <c:v>Late Night (12am-Close)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$3:$T$7</c:f>
+              <c:f>Sheet1!$X$3:$X$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>107050</c:v>
+                  <c:v>80400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1350</c:v>
+                  <c:v>92487.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>124537.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92487.5</c:v>
+                  <c:v>51637.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80400</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1507,9 +1518,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Dates</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1521,12 +1529,40 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1545,7 +1581,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1596,44 +1632,6 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-F4BC-D344-AB2A-2A4AA9FE8ACE}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-F4BC-D344-AB2A-2A4AA9FE8ACE}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>(Sheet1!$B$2,Sheet1!$B$7,Sheet1!$B$12,Sheet1!$B$17,Sheet1!$B$22,Sheet1!$B$27,Sheet1!$B$32,Sheet1!$B$37)</c:f>
@@ -1641,16 +1639,16 @@
                 <c:formatCode>m/d;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>45630</c:v>
+                  <c:v>45357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45647</c:v>
+                  <c:v>45374</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45357</c:v>
+                  <c:v>45448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45374</c:v>
+                  <c:v>45458</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45539</c:v>
@@ -1659,10 +1657,10 @@
                   <c:v>45556</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45448</c:v>
+                  <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45458</c:v>
+                  <c:v>45647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1674,16 +1672,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>49900</c:v>
+                  <c:v>49100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35200</c:v>
+                  <c:v>57200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49100</c:v>
+                  <c:v>51100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57200</c:v>
+                  <c:v>60100</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>46700</c:v>
@@ -1692,10 +1690,10 @@
                   <c:v>63800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51100</c:v>
+                  <c:v>49900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60100</c:v>
+                  <c:v>35200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2028,7 +2026,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
-            <c:idx val="2"/>
+            <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -2042,11 +2040,20 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-AAEF-2E4C-BC58-55EDAA486BBE}"/>
-              </c:ext>
-            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2054,7 +2061,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -2086,44 +2093,6 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-B5F5-D943-B342-F44982E07CB4}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-B5F5-D943-B342-F44982E07CB4}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>(Sheet1!$B$3,Sheet1!$B$8,Sheet1!$B$13,Sheet1!$B$18,Sheet1!$B$23,Sheet1!$B$28,Sheet1!$B$33,Sheet1!$B$38)</c:f>
@@ -2131,16 +2100,16 @@
                 <c:formatCode>m/d;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>45630</c:v>
+                  <c:v>45357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45647</c:v>
+                  <c:v>45374</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45357</c:v>
+                  <c:v>45448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45374</c:v>
+                  <c:v>45458</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45539</c:v>
@@ -2149,10 +2118,10 @@
                   <c:v>45556</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45448</c:v>
+                  <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45458</c:v>
+                  <c:v>45647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2167,13 +2136,13 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1500</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2200</c:v>
+                  <c:v>2700</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2182,10 +2151,10 @@
                   <c:v>3900</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2700</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2581,12 +2550,40 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -2605,7 +2602,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -2656,44 +2653,6 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-C854-3B48-8372-CA129919F55E}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-C854-3B48-8372-CA129919F55E}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>(Sheet1!$B$4,Sheet1!$B$9,Sheet1!$B$14,Sheet1!$B$19,Sheet1!$B$24,Sheet1!$B$29,Sheet1!$B$34,Sheet1!$B$39)</c:f>
@@ -2701,16 +2660,16 @@
                 <c:formatCode>m/d;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>45630</c:v>
+                  <c:v>45357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45647</c:v>
+                  <c:v>45374</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45357</c:v>
+                  <c:v>45448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45374</c:v>
+                  <c:v>45458</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45539</c:v>
@@ -2719,10 +2678,10 @@
                   <c:v>45556</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45448</c:v>
+                  <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45458</c:v>
+                  <c:v>45647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2734,16 +2693,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>168400</c:v>
+                  <c:v>159700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68700</c:v>
+                  <c:v>93300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159700</c:v>
+                  <c:v>163200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93300</c:v>
+                  <c:v>94000</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>157800</c:v>
@@ -2752,10 +2711,10 @@
                   <c:v>91200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163200</c:v>
+                  <c:v>168400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>94000</c:v>
+                  <c:v>68700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3033,12 +2992,40 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -3057,7 +3044,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -3108,44 +3095,6 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-0C72-0048-BB36-C713A94B4676}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-0C72-0048-BB36-C713A94B4676}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>(Sheet1!$B$5,Sheet1!$B$10,Sheet1!$B$15,Sheet1!$B$20,Sheet1!$B$25,Sheet1!$B$30,Sheet1!$B$35,Sheet1!$B$40)</c:f>
@@ -3153,16 +3102,16 @@
                 <c:formatCode>m/d;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>45630</c:v>
+                  <c:v>45357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45647</c:v>
+                  <c:v>45374</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45357</c:v>
+                  <c:v>45448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45374</c:v>
+                  <c:v>45458</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45539</c:v>
@@ -3171,10 +3120,10 @@
                   <c:v>45556</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45448</c:v>
+                  <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45458</c:v>
+                  <c:v>45647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3186,16 +3135,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>93000</c:v>
+                  <c:v>86300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79700</c:v>
+                  <c:v>89800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86300</c:v>
+                  <c:v>96600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89800</c:v>
+                  <c:v>100900</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>87000</c:v>
@@ -3204,10 +3153,10 @@
                   <c:v>106600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96600</c:v>
+                  <c:v>93000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>100900</c:v>
+                  <c:v>79700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3485,12 +3434,40 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="2"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -3509,7 +3486,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -3560,44 +3537,6 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="6"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-1310-AD46-92C0-7076D31C42FB}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="7"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-1310-AD46-92C0-7076D31C42FB}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>(Sheet1!$B$6,Sheet1!$B$11,Sheet1!$B$16,Sheet1!$B$21,Sheet1!$B$26,Sheet1!$B$31,Sheet1!$B$36,Sheet1!$B$41)</c:f>
@@ -3605,16 +3544,16 @@
                 <c:formatCode>m/d;@</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>45630</c:v>
+                  <c:v>45357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45647</c:v>
+                  <c:v>45374</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45357</c:v>
+                  <c:v>45448</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45374</c:v>
+                  <c:v>45458</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45539</c:v>
@@ -3623,10 +3562,10 @@
                   <c:v>45556</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45448</c:v>
+                  <c:v>45630</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45458</c:v>
+                  <c:v>45647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3638,16 +3577,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>143200</c:v>
+                  <c:v>136800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17600</c:v>
+                  <c:v>19200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136800</c:v>
+                  <c:v>141600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19200</c:v>
+                  <c:v>24500</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>136200</c:v>
@@ -3656,10 +3595,10 @@
                   <c:v>24100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>141600</c:v>
+                  <c:v>143200</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24500</c:v>
+                  <c:v>17600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8204,16 +8143,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>238760</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>809340</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>13988</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>695960</xdr:colOff>
+      <xdr:colOff>438279</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>223520</xdr:rowOff>
+      <xdr:rowOff>186708</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8819,10 +8758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CE91CD-F35E-3B47-AC74-378F93CDF0FD}">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8832,7 +8771,7 @@
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8846,18 +8785,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>45630</v>
+        <v>45357</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="4">
-        <v>49900</v>
+        <v>49100</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>11</v>
@@ -8874,19 +8813,19 @@
       <c r="N2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="X2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>45630</v>
+        <v>45357</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -8895,76 +8834,76 @@
         <v>200</v>
       </c>
       <c r="I3">
-        <f>AVERAGE(M3:M6)</f>
-        <v>259050</v>
+        <f>AVERAGE(M3:M5)</f>
+        <v>271433.33333333331</v>
       </c>
       <c r="J3">
-        <f>AVERAGE(N3:N6)</f>
-        <v>430100</v>
+        <f>AVERAGE(N3:N5)</f>
+        <v>437466.66666666669</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M3">
-        <f>SUM(D7:E11)</f>
-        <v>202700</v>
+        <f>SUM(D7:D10)</f>
+        <v>242500</v>
       </c>
       <c r="N3">
         <f>SUM(D2:D6)</f>
-        <v>454700</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T3">
-        <f>AVERAGE(M3:S3,D2,D7,D12,D17,D22,D27,D32,D37)</f>
-        <v>107050</v>
+        <v>432100</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3">
+        <f>AVERAGE(D36,D41,D6,D11,D26,D31,D16,D21)</f>
+        <v>80400</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>45630</v>
+        <v>45357</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4">
-        <v>168400</v>
+        <v>159700</v>
       </c>
       <c r="L4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M4">
-        <f>SUM(D17:E21)</f>
-        <v>261700</v>
+        <f>SUM(D17:D21)</f>
+        <v>282200</v>
       </c>
       <c r="N4">
         <f>SUM(D12:D16)</f>
-        <v>432100</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T4">
-        <f>AVERAGE(D3,D8,D13,D23,D18,D28,D33,D38)</f>
-        <v>1350</v>
+        <v>452600</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="X4">
+        <f>AVERAGE(D35,D40,D5,D10,D25,D30,D15,D20)</f>
+        <v>92487.5</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>45630</v>
+        <v>45357</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4">
-        <v>93000</v>
+        <v>86300</v>
       </c>
       <c r="L5" t="s">
         <v>15</v>
@@ -8974,194 +8913,194 @@
         <v>289600</v>
       </c>
       <c r="N5">
-        <f>SUM(D23:F26)</f>
-        <v>381000</v>
-      </c>
-      <c r="R5" s="4" t="s">
+        <f>SUM(D22:D26)</f>
+        <v>427700</v>
+      </c>
+      <c r="V5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="T5">
-        <f>AVERAGE(D4,D9,D14,D19,D24,D29,D34,D39)</f>
+      <c r="X5">
+        <f>AVERAGE(D34,D39,D4,D9,D24,D29,D14,D19)</f>
         <v>124537.5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>45630</v>
+        <v>45357</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4">
-        <v>143200</v>
+        <v>136800</v>
       </c>
       <c r="L6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M6">
         <f>SUM(D37:D41)</f>
-        <v>282200</v>
+        <v>202700</v>
       </c>
       <c r="N6">
         <f>SUM(D32:D36)</f>
-        <v>452600</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="T6">
-        <f>AVERAGE(D5,D10,D15,D20,D25,D30,D35,D40)</f>
-        <v>92487.5</v>
+        <v>454700</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X6">
+        <f>AVERAGE(O3:S3,D32,D37,D2,D7,D22,D27,D12,D17)</f>
+        <v>51637.5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>45647</v>
+        <v>45374</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>35200</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="T7">
-        <f>AVERAGE(D6,D11,D16,D21,D26,D31,D36,D41)</f>
-        <v>80400</v>
+        <v>57200</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <f>AVERAGE(D33,D38,D3,D23,D8,D28,D13,D18)</f>
+        <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>45647</v>
+        <v>45374</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4">
-        <v>1500</v>
+        <v>2200</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>45647</v>
+        <v>45374</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="4">
-        <v>68700</v>
+        <v>93300</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>45647</v>
+        <v>45374</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="4">
-        <v>79700</v>
+        <v>89800</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="6">
-        <v>45647</v>
+        <v>45374</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4">
-        <v>17600</v>
+        <v>19200</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>45357</v>
-      </c>
-      <c r="C12" s="4" t="s">
+        <v>45448</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="4">
-        <v>49100</v>
+      <c r="D12" s="1">
+        <v>51100</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>45357</v>
-      </c>
-      <c r="C13" s="4" t="s">
+        <v>45448</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="4">
-        <v>200</v>
+      <c r="D13" s="1">
+        <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>45357</v>
-      </c>
-      <c r="C14" s="4" t="s">
+        <v>45448</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="4">
-        <v>159700</v>
+      <c r="D14" s="1">
+        <v>163200</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>45357</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>45448</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="4">
-        <v>86300</v>
+      <c r="D15" s="1">
+        <v>96600</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>45357</v>
-      </c>
-      <c r="C16" s="4" t="s">
+        <v>45448</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="4">
-        <v>136800</v>
+      <c r="D16" s="1">
+        <v>141600</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9169,13 +9108,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="6">
-        <v>45374</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>45458</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
-        <v>57200</v>
+      <c r="D17" s="1">
+        <v>60100</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9183,13 +9122,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>45374</v>
-      </c>
-      <c r="C18" s="4" t="s">
+        <v>45458</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="4">
-        <v>2200</v>
+      <c r="D18" s="1">
+        <v>2700</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9197,13 +9136,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>45374</v>
-      </c>
-      <c r="C19" s="4" t="s">
+        <v>45458</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="4">
-        <v>93300</v>
+      <c r="D19" s="1">
+        <v>94000</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9211,13 +9150,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>45374</v>
-      </c>
-      <c r="C20" s="4" t="s">
+        <v>45458</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="4">
-        <v>89800</v>
+      <c r="D20" s="1">
+        <v>100900</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9225,13 +9164,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>45374</v>
-      </c>
-      <c r="C21" s="4" t="s">
+        <v>45458</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="4">
-        <v>19200</v>
+      <c r="D21" s="1">
+        <v>24500</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9379,13 +9318,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="6">
-        <v>45448</v>
-      </c>
-      <c r="C32" s="1" t="s">
+        <v>45630</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="1">
-        <v>51100</v>
+      <c r="D32" s="4">
+        <v>49900</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9393,13 +9332,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="6">
-        <v>45448</v>
-      </c>
-      <c r="C33" s="1" t="s">
+        <v>45630</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="1">
-        <v>100</v>
+      <c r="D33" s="4">
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9407,13 +9346,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="6">
-        <v>45448</v>
-      </c>
-      <c r="C34" s="1" t="s">
+        <v>45630</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="1">
-        <v>163200</v>
+      <c r="D34" s="4">
+        <v>168400</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9421,13 +9360,13 @@
         <v>33</v>
       </c>
       <c r="B35" s="6">
-        <v>45448</v>
-      </c>
-      <c r="C35" s="1" t="s">
+        <v>45630</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="1">
-        <v>96600</v>
+      <c r="D35" s="4">
+        <v>93000</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9435,13 +9374,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="6">
-        <v>45448</v>
-      </c>
-      <c r="C36" s="1" t="s">
+        <v>45630</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="1">
-        <v>141600</v>
+      <c r="D36" s="4">
+        <v>143200</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9449,13 +9388,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="6">
-        <v>45458</v>
-      </c>
-      <c r="C37" s="1" t="s">
+        <v>45647</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="1">
-        <v>60100</v>
+      <c r="D37" s="4">
+        <v>35200</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9463,13 +9402,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="6">
-        <v>45458</v>
-      </c>
-      <c r="C38" s="1" t="s">
+        <v>45647</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="1">
-        <v>2700</v>
+      <c r="D38" s="4">
+        <v>1500</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9477,13 +9416,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="6">
-        <v>45458</v>
-      </c>
-      <c r="C39" s="1" t="s">
+        <v>45647</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="1">
-        <v>94000</v>
+      <c r="D39" s="4">
+        <v>68700</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9491,13 +9430,13 @@
         <v>38</v>
       </c>
       <c r="B40" s="6">
-        <v>45458</v>
-      </c>
-      <c r="C40" s="1" t="s">
+        <v>45647</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="1">
-        <v>100900</v>
+      <c r="D40" s="4">
+        <v>79700</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -9505,13 +9444,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="6">
-        <v>45458</v>
-      </c>
-      <c r="C41" s="1" t="s">
+        <v>45647</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="1">
-        <v>24500</v>
+      <c r="D41" s="4">
+        <v>17600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>